<commit_message>
Agora o arquivo abre sozinho
</commit_message>
<xml_diff>
--- a/DemonstrativoFinanceiro.xlsx
+++ b/DemonstrativoFinanceiro.xlsx
@@ -685,7 +685,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -718,7 +718,7 @@
       </c>
       <c r="B2" s="24" t="inlineStr">
         <is>
-          <t>R$615.35</t>
+          <t>R$100.00</t>
         </is>
       </c>
       <c r="C2" s="1" t="n"/>
@@ -726,7 +726,7 @@
     <row r="3">
       <c r="A3" s="25" t="inlineStr">
         <is>
-          <t>03-2024</t>
+          <t>04-2024</t>
         </is>
       </c>
     </row>
@@ -756,7 +756,7 @@
       </c>
       <c r="B5" s="26" t="inlineStr">
         <is>
-          <t>R$100.00</t>
+          <t>R$233.00</t>
         </is>
       </c>
       <c r="C5" s="27" t="inlineStr"/>
@@ -769,7 +769,7 @@
       </c>
       <c r="B6" s="26" t="inlineStr">
         <is>
-          <t>R$100.00</t>
+          <t>R$233.00</t>
         </is>
       </c>
       <c r="C6" s="27" t="inlineStr"/>
@@ -782,7 +782,7 @@
       </c>
       <c r="B7" s="26" t="inlineStr">
         <is>
-          <t>R$100.00</t>
+          <t>R$233.00</t>
         </is>
       </c>
       <c r="C7" s="27" t="inlineStr"/>
@@ -795,7 +795,7 @@
       </c>
       <c r="B8" s="26" t="inlineStr">
         <is>
-          <t>R$100.00</t>
+          <t>R$233.00</t>
         </is>
       </c>
       <c r="C8" s="27" t="inlineStr"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="B9" s="26" t="inlineStr">
         <is>
-          <t>R$100.00</t>
+          <t>R$233.00</t>
         </is>
       </c>
       <c r="C9" s="27" t="inlineStr"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="B10" s="26" t="inlineStr">
         <is>
-          <t>R$100.00</t>
+          <t>R$233.00</t>
         </is>
       </c>
       <c r="C10" s="27" t="inlineStr"/>
@@ -834,7 +834,7 @@
       </c>
       <c r="B12" s="14" t="inlineStr">
         <is>
-          <t>R$600.00</t>
+          <t>R$1398.00</t>
         </is>
       </c>
       <c r="C12" s="13" t="n"/>
@@ -859,135 +859,111 @@
     <row r="15">
       <c r="A15" s="28" t="inlineStr">
         <is>
-          <t>Copasa</t>
+          <t>copasa</t>
         </is>
       </c>
       <c r="B15" s="29" t="inlineStr">
         <is>
-          <t>R$475.24</t>
+          <t>R$100.00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="28" t="inlineStr">
         <is>
-          <t>Cemig</t>
+          <t>skdks</t>
         </is>
       </c>
       <c r="B16" s="29" t="inlineStr">
         <is>
-          <t>R$86.20</t>
+          <t>R$232.00</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="28" t="inlineStr">
-        <is>
-          <t>Cera</t>
-        </is>
-      </c>
-      <c r="B17" s="29" t="inlineStr">
-        <is>
-          <t>R$11.80</t>
-        </is>
-      </c>
+      <c r="A17" s="6" t="n"/>
+      <c r="B17" s="21" t="n"/>
+      <c r="C17" s="6" t="n"/>
     </row>
     <row r="18" ht="23.25" customHeight="1">
-      <c r="A18" s="28" t="inlineStr">
-        <is>
-          <t>Randup</t>
-        </is>
-      </c>
-      <c r="B18" s="29" t="inlineStr">
-        <is>
-          <t>R$60.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="n"/>
-      <c r="B19" s="21" t="n"/>
-      <c r="C19" s="6" t="n"/>
-    </row>
+      <c r="A18" s="18" t="inlineStr">
+        <is>
+          <t>Total de Despesas:</t>
+        </is>
+      </c>
+      <c r="B18" s="19" t="inlineStr">
+        <is>
+          <t>R$332.00</t>
+        </is>
+      </c>
+      <c r="C18" s="20" t="n"/>
+    </row>
+    <row r="19"/>
     <row r="20">
-      <c r="A20" s="18" t="inlineStr">
-        <is>
-          <t>Total de Despesas:</t>
-        </is>
-      </c>
-      <c r="B20" s="19" t="inlineStr">
-        <is>
-          <t>R$633.24</t>
-        </is>
-      </c>
-      <c r="C20" s="20" t="n"/>
-    </row>
-    <row r="21"/>
+      <c r="A20" s="15" t="inlineStr">
+        <is>
+          <t>3-Resumo Financeiro</t>
+        </is>
+      </c>
+      <c r="B20" s="16" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+      <c r="C20" s="17" t="inlineStr">
+        <is>
+          <t>Mês em Atraso</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>Saldo Mês anterior:</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>R$100.00</t>
+        </is>
+      </c>
+      <c r="C21" s="6" t="n"/>
+    </row>
     <row r="22">
-      <c r="A22" s="15" t="inlineStr">
-        <is>
-          <t>3-Resumo Financeiro</t>
-        </is>
-      </c>
-      <c r="B22" s="16" t="inlineStr">
-        <is>
-          <t>Valor</t>
-        </is>
-      </c>
-      <c r="C22" s="17" t="inlineStr">
-        <is>
-          <t>Mês em Atraso</t>
-        </is>
-      </c>
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t>Receitas Realizadas:</t>
+        </is>
+      </c>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>R$1398.00</t>
+        </is>
+      </c>
+      <c r="C22" s="6" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="10" t="inlineStr">
         <is>
-          <t>Saldo Mês anterior:</t>
+          <t>Despesas Realizadas</t>
         </is>
       </c>
       <c r="B23" s="6" t="inlineStr">
         <is>
-          <t>R$615.35</t>
+          <t>R$332.00</t>
         </is>
       </c>
       <c r="C23" s="6" t="n"/>
     </row>
-    <row r="24">
-      <c r="A24" s="10" t="inlineStr">
-        <is>
-          <t>Receitas Realizadas:</t>
-        </is>
-      </c>
-      <c r="B24" s="6" t="inlineStr">
-        <is>
-          <t>R$600.00</t>
-        </is>
-      </c>
-      <c r="C24" s="6" t="n"/>
-    </row>
     <row r="25">
-      <c r="A25" s="10" t="inlineStr">
-        <is>
-          <t>Despesas Realizadas</t>
-        </is>
-      </c>
-      <c r="B25" s="6" t="inlineStr">
-        <is>
-          <t>R$633.24</t>
-        </is>
-      </c>
-      <c r="C25" s="6" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="30" t="inlineStr">
+      <c r="A25" s="30" t="inlineStr">
         <is>
           <t>Saldo Atual:</t>
         </is>
       </c>
-      <c r="B27" s="31" t="inlineStr">
-        <is>
-          <t>R$582.11</t>
+      <c r="B25" s="31" t="inlineStr">
+        <is>
+          <t>R$1166.0</t>
         </is>
       </c>
     </row>

</xml_diff>